<commit_message>
xlxs with date asstring / xlxs con fecha en formato texto
</commit_message>
<xml_diff>
--- a/20160321_data_sets_V2.xlsx
+++ b/20160321_data_sets_V2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\local\dev\Diagnostics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Health Sciences\CIS\data\Diagnostics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -208,7 +208,94 @@
     <t>^ must contain letters</t>
   </si>
   <si>
-    <t>wfwqe 10/10/15</t>
+    <t>sep 15</t>
+  </si>
+  <si>
+    <t>aug 15</t>
+  </si>
+  <si>
+    <t>jul 15</t>
+  </si>
+  <si>
+    <t>jun 15</t>
+  </si>
+  <si>
+    <t>may 15</t>
+  </si>
+  <si>
+    <t>apr 15</t>
+  </si>
+  <si>
+    <t>mar 15</t>
+  </si>
+  <si>
+    <t>feb 15</t>
+  </si>
+  <si>
+    <t>jan 15</t>
+  </si>
+  <si>
+    <t>dec 14</t>
+  </si>
+  <si>
+    <t>nov 14</t>
+  </si>
+  <si>
+    <t>oct 14</t>
+  </si>
+  <si>
+    <t>sep 14</t>
+  </si>
+  <si>
+    <t>aug 14</t>
+  </si>
+  <si>
+    <t>jul 14</t>
+  </si>
+  <si>
+    <t>jun 14</t>
+  </si>
+  <si>
+    <t>may 14</t>
+  </si>
+  <si>
+    <t>apr 14</t>
+  </si>
+  <si>
+    <t>mar 14</t>
+  </si>
+  <si>
+    <t>feb 14</t>
+  </si>
+  <si>
+    <t>jan 14</t>
+  </si>
+  <si>
+    <t>dec 12</t>
+  </si>
+  <si>
+    <t>nov 12</t>
+  </si>
+  <si>
+    <t>oct 12</t>
+  </si>
+  <si>
+    <t>sep 12</t>
+  </si>
+  <si>
+    <t>aug 12</t>
+  </si>
+  <si>
+    <t>jul 12</t>
+  </si>
+  <si>
+    <t>jun 12</t>
+  </si>
+  <si>
+    <t>may 12</t>
+  </si>
+  <si>
+    <t>apr 12</t>
   </si>
 </sst>
 </file>
@@ -1020,13 +1107,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="146.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1127,9 +1217,6 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1164,7 +1251,7 @@
         <v>60</v>
       </c>
       <c r="B9" s="1">
-        <v>42248</v>
+        <v>42278</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -1174,8 +1261,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>201509</v>
+      <c r="A10" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="B10" s="1">
         <v>42248</v>
@@ -1188,8 +1275,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>201508</v>
+      <c r="A11" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="B11" s="1">
         <v>42217</v>
@@ -1202,8 +1289,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>201507</v>
+      <c r="A12" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="B12" s="1">
         <v>42186</v>
@@ -1216,8 +1303,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>201506</v>
+      <c r="A13" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="B13" s="1">
         <v>42156</v>
@@ -1230,8 +1317,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>201505</v>
+      <c r="A14" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="B14" s="1">
         <v>42125</v>
@@ -1244,8 +1331,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>201504</v>
+      <c r="A15" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B15" s="1">
         <v>42095</v>
@@ -1258,8 +1345,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>201503</v>
+      <c r="A16" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="B16" s="1">
         <v>42064</v>
@@ -1272,8 +1359,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>201502</v>
+      <c r="A17" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="B17" s="1">
         <v>42036</v>
@@ -1286,8 +1373,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>201501</v>
+      <c r="A18" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B18" s="1">
         <v>42005</v>
@@ -1300,8 +1387,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>201412</v>
+      <c r="A19" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B19" s="1">
         <v>41974</v>
@@ -1314,8 +1401,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>201411</v>
+      <c r="A20" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B20" s="1">
         <v>41944</v>
@@ -1328,8 +1415,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>201410</v>
+      <c r="A21" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B21" s="1">
         <v>41913</v>
@@ -1342,8 +1429,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>201409</v>
+      <c r="A22" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B22" s="1">
         <v>41883</v>
@@ -1356,8 +1443,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>201408</v>
+      <c r="A23" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="B23" s="1">
         <v>41852</v>
@@ -1370,8 +1457,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>201407</v>
+      <c r="A24" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B24" s="1">
         <v>41821</v>
@@ -1384,8 +1471,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>201406</v>
+      <c r="A25" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B25" s="1">
         <v>41791</v>
@@ -1398,8 +1485,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>201405</v>
+      <c r="A26" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B26" s="1">
         <v>41760</v>
@@ -1412,8 +1499,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>201404</v>
+      <c r="A27" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="B27" s="1">
         <v>41730</v>
@@ -1426,8 +1513,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>201403</v>
+      <c r="A28" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="B28" s="1">
         <v>41699</v>
@@ -1440,8 +1527,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>201402</v>
+      <c r="A29" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="B29" s="1">
         <v>41671</v>
@@ -1454,8 +1541,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>201401</v>
+      <c r="A30" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="B30" s="1">
         <v>41640</v>
@@ -1468,8 +1555,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>201312</v>
+      <c r="A31" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="B31" s="1">
         <v>41609</v>
@@ -1482,8 +1569,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>201311</v>
+      <c r="A32" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B32" s="1">
         <v>41579</v>
@@ -1496,8 +1583,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>201310</v>
+      <c r="A33" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B33" s="1">
         <v>41548</v>
@@ -1510,8 +1597,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>201309</v>
+      <c r="A34" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="B34" s="1">
         <v>41518</v>
@@ -1524,8 +1611,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>201308</v>
+      <c r="A35" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="B35" s="1">
         <v>41487</v>
@@ -1538,8 +1625,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>201307</v>
+      <c r="A36" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="B36" s="1">
         <v>41456</v>
@@ -1552,8 +1639,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>201306</v>
+      <c r="A37" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B37" s="1">
         <v>41426</v>
@@ -1566,8 +1653,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>201305</v>
+      <c r="A38" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="B38" s="1">
         <v>41395</v>
@@ -1580,8 +1667,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>201304</v>
+      <c r="A39" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="B39" s="1">
         <v>41365</v>

</xml_diff>

<commit_message>
new xlxs with date as string (yyyymm) / nuevo xlxs con fecha en formato texto (aaaamm)
</commit_message>
<xml_diff>
--- a/20160321_data_sets_V2.xlsx
+++ b/20160321_data_sets_V2.xlsx
@@ -193,109 +193,109 @@
     <t>^ if null then enter date 1-1-1</t>
   </si>
   <si>
-    <t>dec 15</t>
-  </si>
-  <si>
-    <t>jan 16</t>
-  </si>
-  <si>
-    <t>nov 15</t>
-  </si>
-  <si>
-    <t>oct 15</t>
-  </si>
-  <si>
     <t>^ must contain letters</t>
   </si>
   <si>
-    <t>sep 15</t>
-  </si>
-  <si>
-    <t>aug 15</t>
-  </si>
-  <si>
-    <t>jul 15</t>
-  </si>
-  <si>
-    <t>jun 15</t>
-  </si>
-  <si>
-    <t>may 15</t>
-  </si>
-  <si>
-    <t>apr 15</t>
-  </si>
-  <si>
-    <t>mar 15</t>
-  </si>
-  <si>
-    <t>feb 15</t>
-  </si>
-  <si>
-    <t>jan 15</t>
-  </si>
-  <si>
-    <t>dec 14</t>
-  </si>
-  <si>
-    <t>nov 14</t>
-  </si>
-  <si>
-    <t>oct 14</t>
-  </si>
-  <si>
-    <t>sep 14</t>
-  </si>
-  <si>
-    <t>aug 14</t>
-  </si>
-  <si>
-    <t>jul 14</t>
-  </si>
-  <si>
-    <t>jun 14</t>
-  </si>
-  <si>
-    <t>may 14</t>
-  </si>
-  <si>
-    <t>apr 14</t>
-  </si>
-  <si>
-    <t>mar 14</t>
-  </si>
-  <si>
-    <t>feb 14</t>
-  </si>
-  <si>
-    <t>jan 14</t>
-  </si>
-  <si>
-    <t>dec 12</t>
-  </si>
-  <si>
-    <t>nov 12</t>
-  </si>
-  <si>
-    <t>oct 12</t>
-  </si>
-  <si>
-    <t>sep 12</t>
-  </si>
-  <si>
-    <t>aug 12</t>
-  </si>
-  <si>
-    <t>jul 12</t>
-  </si>
-  <si>
-    <t>jun 12</t>
-  </si>
-  <si>
-    <t>may 12</t>
-  </si>
-  <si>
-    <t>apr 12</t>
+    <t>201601</t>
+  </si>
+  <si>
+    <t>201512</t>
+  </si>
+  <si>
+    <t>201511</t>
+  </si>
+  <si>
+    <t>201510</t>
+  </si>
+  <si>
+    <t>201509</t>
+  </si>
+  <si>
+    <t>201508</t>
+  </si>
+  <si>
+    <t>201507</t>
+  </si>
+  <si>
+    <t>201506</t>
+  </si>
+  <si>
+    <t>201505</t>
+  </si>
+  <si>
+    <t>201504</t>
+  </si>
+  <si>
+    <t>201503</t>
+  </si>
+  <si>
+    <t>201502</t>
+  </si>
+  <si>
+    <t>201501</t>
+  </si>
+  <si>
+    <t>201412</t>
+  </si>
+  <si>
+    <t>201411</t>
+  </si>
+  <si>
+    <t>201410</t>
+  </si>
+  <si>
+    <t>201409</t>
+  </si>
+  <si>
+    <t>201408</t>
+  </si>
+  <si>
+    <t>201407</t>
+  </si>
+  <si>
+    <t>201406</t>
+  </si>
+  <si>
+    <t>201405</t>
+  </si>
+  <si>
+    <t>201404</t>
+  </si>
+  <si>
+    <t>201403</t>
+  </si>
+  <si>
+    <t>201402</t>
+  </si>
+  <si>
+    <t>201401</t>
+  </si>
+  <si>
+    <t>201312</t>
+  </si>
+  <si>
+    <t>201311</t>
+  </si>
+  <si>
+    <t>201310</t>
+  </si>
+  <si>
+    <t>201309</t>
+  </si>
+  <si>
+    <t>201308</t>
+  </si>
+  <si>
+    <t>201307</t>
+  </si>
+  <si>
+    <t>201306</t>
+  </si>
+  <si>
+    <t>201305</t>
+  </si>
+  <si>
+    <t>201304</t>
   </si>
 </sst>
 </file>
@@ -1107,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,6 +1117,7 @@
     <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="146.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1220,7 +1221,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1">
         <v>42339</v>
@@ -1234,7 +1235,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1">
         <v>42309</v>
@@ -1248,7 +1249,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1">
         <v>42278</v>
@@ -1683,6 +1684,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A6:A18 A19:A30 A31:A39" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1745,7 +1749,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>